<commit_message>
📈 Output aggiornato automaticamente
</commit_message>
<xml_diff>
--- a/output/dati_azioni_completo_2025-05-29.xlsx
+++ b/output/dati_azioni_completo_2025-05-29.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO7"/>
+  <dimension ref="A1:AP7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,195 +450,200 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Shares Outstanding</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Float Shares</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Insider Ownership</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Institutional Ownership</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Open</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Prev Close</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Close</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Gap %</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>VWAP</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>VWAP %</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>High Pre-Market</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Open vs Pre-Market %</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>High_1m</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Low_1m</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Volume_1m</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Break_PMH_1m</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>High_5m</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Low_5m</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Volume_5m</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Break_PMH_5m</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>High_30m</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Low_30m</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Volume_30m</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Break_PMH_30m</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>High_1h</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Low_1h</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Volume_1h</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Break_PMH_1h</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>High_90m</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Low_90m</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Volume_90m</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Break_PMH_90m</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>High_4h</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Low_4h</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Volume_4h</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Break_PMH_4h</t>
         </is>
@@ -654,126 +659,129 @@
         <v>3987824</v>
       </c>
       <c r="C2" t="n">
+        <v>733056</v>
+      </c>
+      <c r="D2" t="n">
         <v>715917</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.03221</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.00877</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>45806</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>7.760000228881836</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>3.319999933242798</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>8.220000267028809</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>5.210000038146973</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>5.440000057220459</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>77704200</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>134</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>7.08</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>-8.81</v>
       </c>
-      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="n">
         <v>5.93</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>-32.86</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>77363199</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="V2" t="n">
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W2" t="n">
         <v>5.93</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>-32.86</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Y2" t="n">
         <v>77363199</v>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Z2" t="n">
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AA2" t="n">
         <v>5.93</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>-32.86</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>77363199</v>
       </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AD2" t="n">
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AE2" t="n">
         <v>5.93</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AF2" t="n">
         <v>-32.86</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AG2" t="n">
         <v>77363199</v>
       </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AH2" t="n">
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AI2" t="n">
         <v>5.93</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AJ2" t="n">
         <v>-32.86</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AK2" t="n">
         <v>77363199</v>
       </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AL2" t="n">
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AM2" t="n">
         <v>5.93</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AN2" t="n">
         <v>-32.86</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AO2" t="n">
         <v>77363199</v>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
@@ -789,126 +797,129 @@
         <v>27544554</v>
       </c>
       <c r="C3" t="n">
+        <v>5923560</v>
+      </c>
+      <c r="D3" t="n">
         <v>5237729</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.11578</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.19909</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="G3" s="2" t="n">
         <v>45806</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>5.119999885559082</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>3.880000114440918</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>5.5</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>4.269999980926514</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>4.650000095367432</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>6868800</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>32</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>5.02</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>-1.89</v>
       </c>
-      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="n">
         <v>7.42</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>-16.6</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>6858369</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="V3" t="n">
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
         <v>7.42</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>-16.6</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Y3" t="n">
         <v>6826231</v>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Z3" t="n">
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AA3" t="n">
         <v>7.42</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>-16.6</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>6826231</v>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AD3" t="n">
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AE3" t="n">
         <v>7.42</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AF3" t="n">
         <v>-16.6</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AG3" t="n">
         <v>6826231</v>
       </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AH3" t="n">
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AI3" t="n">
         <v>7.42</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AJ3" t="n">
         <v>-16.6</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AK3" t="n">
         <v>6826231</v>
       </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AL3" t="n">
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AM3" t="n">
         <v>7.42</v>
       </c>
-      <c r="AM3" t="n">
+      <c r="AN3" t="n">
         <v>-16.6</v>
       </c>
-      <c r="AN3" t="n">
+      <c r="AO3" t="n">
         <v>6826231</v>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="AP3" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
@@ -924,126 +935,129 @@
         <v>3231050</v>
       </c>
       <c r="C4" t="n">
+        <v>2584840</v>
+      </c>
+      <c r="D4" t="n">
         <v>2142673</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.03482</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.02309</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="G4" s="2" t="n">
         <v>45806</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>1.240000009536743</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.8560000061988831</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>1.389999985694885</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>1.039999961853027</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>1.25</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>41865200</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>45</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>1.24</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>0.39</v>
       </c>
-      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="n">
         <v>12.1</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>-16.13</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>41448944</v>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="V4" t="n">
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W4" t="n">
         <v>12.1</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>-16.13</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Y4" t="n">
         <v>41448149</v>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Z4" t="n">
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AA4" t="n">
         <v>12.1</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>-16.13</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>41448149</v>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AD4" t="n">
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AE4" t="n">
         <v>12.1</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AF4" t="n">
         <v>-16.13</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AG4" t="n">
         <v>41448149</v>
       </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AH4" t="n">
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AI4" t="n">
         <v>12.1</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AJ4" t="n">
         <v>-16.13</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AK4" t="n">
         <v>41448149</v>
       </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AL4" t="n">
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AM4" t="n">
         <v>12.1</v>
       </c>
-      <c r="AM4" t="n">
+      <c r="AN4" t="n">
         <v>-16.13</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AO4" t="n">
         <v>41448149</v>
       </c>
-      <c r="AO4" t="inlineStr">
+      <c r="AP4" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
@@ -1059,126 +1073,129 @@
         <v>22436236</v>
       </c>
       <c r="C5" t="n">
+        <v>4331320</v>
+      </c>
+      <c r="D5" t="n">
         <v>21867326</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.17916</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.16569</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="G5" s="2" t="n">
         <v>45806</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>5.039999961853027</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>2.289999961853027</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>5.199999809265137</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>4.940000057220459</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>5.179999828338623</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>3003600</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>120</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>5.09</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>0.9</v>
       </c>
-      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="n">
         <v>3.17</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>-1.98</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>2974680</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="V5" t="n">
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W5" t="n">
         <v>3.17</v>
       </c>
-      <c r="W5" t="n">
+      <c r="X5" t="n">
         <v>-1.98</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Y5" t="n">
         <v>2968967</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Z5" t="n">
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AA5" t="n">
         <v>3.17</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>-1.98</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>2968967</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AD5" t="n">
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AE5" t="n">
         <v>3.17</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AF5" t="n">
         <v>-1.98</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AG5" t="n">
         <v>2968967</v>
       </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AH5" t="n">
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AI5" t="n">
         <v>3.17</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AJ5" t="n">
         <v>-1.98</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AK5" t="n">
         <v>2968967</v>
       </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AL5" t="n">
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AM5" t="n">
         <v>3.17</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AN5" t="n">
         <v>-1.98</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AO5" t="n">
         <v>2968967</v>
       </c>
-      <c r="AO5" t="inlineStr">
+      <c r="AP5" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
@@ -1194,126 +1211,129 @@
         <v>72820000</v>
       </c>
       <c r="C6" t="n">
+        <v>22000000</v>
+      </c>
+      <c r="D6" t="n">
         <v>5381600</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.74088997</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.00088</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="G6" s="2" t="n">
         <v>45806</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>3.869999885559082</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>1.960000038146973</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>4.25</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>2.269999980926514</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>3.309999942779541</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>27500500</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>97</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>3.32</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>-14.31</v>
       </c>
-      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="n">
         <v>9.82</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>-41.34</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>26800547</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="V6" t="n">
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W6" t="n">
         <v>9.82</v>
       </c>
-      <c r="W6" t="n">
+      <c r="X6" t="n">
         <v>-41.34</v>
       </c>
-      <c r="X6" t="n">
+      <c r="Y6" t="n">
         <v>26798765</v>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Z6" t="n">
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AA6" t="n">
         <v>9.82</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AB6" t="n">
         <v>-41.34</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>26798765</v>
       </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AD6" t="n">
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AE6" t="n">
         <v>9.82</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AF6" t="n">
         <v>-41.34</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AG6" t="n">
         <v>26798765</v>
       </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AH6" t="n">
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AI6" t="n">
         <v>9.82</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AJ6" t="n">
         <v>-41.34</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AK6" t="n">
         <v>26798765</v>
       </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AL6" t="n">
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AM6" t="n">
         <v>9.82</v>
       </c>
-      <c r="AM6" t="n">
+      <c r="AN6" t="n">
         <v>-41.34</v>
       </c>
-      <c r="AN6" t="n">
+      <c r="AO6" t="n">
         <v>26798765</v>
       </c>
-      <c r="AO6" t="inlineStr">
+      <c r="AP6" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
@@ -1329,126 +1349,129 @@
         <v>440806464</v>
       </c>
       <c r="C7" t="n">
+        <v>14031300</v>
+      </c>
+      <c r="D7" t="n">
         <v>6891600</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.23892</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.62556</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="G7" s="2" t="n">
         <v>45806</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>2.849999904632568</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>1.580000042915344</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>3.470000028610229</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>2.630000114440918</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>3.430000066757202</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>104632200</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>80</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>2.91</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>2.03</v>
       </c>
-      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="n">
         <v>21.75</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>-7.72</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>103390767</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="V7" t="n">
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="W7" t="n">
         <v>21.75</v>
       </c>
-      <c r="W7" t="n">
+      <c r="X7" t="n">
         <v>-7.72</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Y7" t="n">
         <v>103390767</v>
       </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Z7" t="n">
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AA7" t="n">
         <v>21.75</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AB7" t="n">
         <v>-7.72</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>103390767</v>
       </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AD7" t="n">
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AE7" t="n">
         <v>21.75</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AF7" t="n">
         <v>-7.72</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AG7" t="n">
         <v>103390767</v>
       </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AH7" t="n">
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AI7" t="n">
         <v>21.75</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AJ7" t="n">
         <v>-7.72</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AK7" t="n">
         <v>103390767</v>
       </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="AL7" t="n">
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="AM7" t="n">
         <v>21.75</v>
       </c>
-      <c r="AM7" t="n">
+      <c r="AN7" t="n">
         <v>-7.72</v>
       </c>
-      <c r="AN7" t="n">
+      <c r="AO7" t="n">
         <v>103390767</v>
       </c>
-      <c r="AO7" t="inlineStr">
+      <c r="AP7" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>

</xml_diff>